<commit_message>
included BDI header options and cable options
</commit_message>
<xml_diff>
--- a/puntos_1.xlsx
+++ b/puntos_1.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AZ14"/>
+  <dimension ref="A1:AZ16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,17 +432,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1 SU col</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-57.75229665737701</t>
+          <t>-57.75526384350523</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-30.86397242051519</t>
+          <t>-30.84392242816692</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -452,24 +452,24 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>S30.863972° W57.752296°</t>
+          <t>S30.843922° W57.755263°</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2 AA BA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-57.75285839699505</t>
+          <t>-57.75428294205687</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-30.85975540560617</t>
+          <t>-30.84993317123787</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -479,24 +479,24 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>S30.859755° W57.752858°</t>
+          <t>S30.849933° W57.754282°</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3 SA RD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-57.75526384350523</t>
+          <t>-57.75354348580155</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-30.84392242816692</t>
+          <t>-30.85513424867982</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -506,24 +506,24 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>S30.843922° W57.755263°</t>
+          <t>S30.855134° W57.753543°</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4 AA DE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-57.75354348580155</t>
+          <t>-57.75285839699505</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-30.85513424867982</t>
+          <t>-30.85975540560617</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -533,24 +533,24 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>S30.855134° W57.753543°</t>
+          <t>S30.859755° W57.752858°</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-57.75428294205687</t>
+          <t>-57.75229665737701</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-30.84993317123787</t>
+          <t>-30.86397242051519</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -560,751 +560,805 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>S30.849933° W57.754282°</t>
+          <t>S30.863972° W57.752296°</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Lines</t>
+          <t>6 col</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>-57.74385608985</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-30.85955381593797</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>S30.859553° W57.743856°</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>waypoints1</t>
+          <t>7 Col</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>waypoints1_1</t>
+          <t>-57.75022047957408</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-57.74591030449292</t>
+          <t>-30.85069516230872</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>-30.84191223192256</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>waypoints1_2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-57.7328311040636</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-30.84814365439827</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>waypoints1_3</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>-57.73314345725397</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>-30.8539877149353</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>waypoints1_4</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>-57.73542685741717</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>-30.86169653128272</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>waypoints1_5</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>-57.7408503849196</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>-30.86035901665188</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>waypoints1_6</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>-57.73549932725664</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>-30.85579893507902</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>waypoints1_7</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>-57.74177445486709</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>-30.85506639734164</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>waypoints1_8</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>-57.7355574257188</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>-30.85281788159316</t>
-        </is>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>-57.74124633025218</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>-30.85041651641221</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>waypoints1_10</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>-57.74690239008397</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>-30.85374166882512</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>waypoints1_11</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>-57.74701342335079</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>-30.85384714723152</t>
-        </is>
-      </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>waypoints1_12</t>
-        </is>
-      </c>
-      <c r="AJ8" t="inlineStr">
-        <is>
-          <t>-57.74906400692047</t>
-        </is>
-      </c>
-      <c r="AK8" t="inlineStr">
-        <is>
-          <t>-30.8481931267192</t>
-        </is>
-      </c>
-      <c r="AL8" t="inlineStr">
-        <is>
-          <t>waypoints1_13</t>
-        </is>
-      </c>
-      <c r="AM8" t="inlineStr">
-        <is>
-          <t>-57.74462108277138</t>
-        </is>
-      </c>
-      <c r="AN8" t="inlineStr">
-        <is>
-          <t>-30.84793624415745</t>
-        </is>
-      </c>
-      <c r="AO8" t="inlineStr">
-        <is>
-          <t>waypoints1_14</t>
-        </is>
-      </c>
-      <c r="AP8" t="inlineStr">
-        <is>
-          <t>-57.74887913878435</t>
-        </is>
-      </c>
-      <c r="AQ8" t="inlineStr">
-        <is>
-          <t>-30.84464624755162</t>
-        </is>
-      </c>
-      <c r="AR8" t="inlineStr">
-        <is>
-          <t>waypoints1_15</t>
-        </is>
-      </c>
-      <c r="AS8" t="inlineStr">
-        <is>
-          <t>-57.73937946143569</t>
-        </is>
-      </c>
-      <c r="AT8" t="inlineStr">
-        <is>
-          <t>-30.84663672177698</t>
-        </is>
-      </c>
-      <c r="AU8" t="inlineStr">
-        <is>
-          <t>waypoints1_16</t>
-        </is>
-      </c>
-      <c r="AV8" t="inlineStr">
-        <is>
-          <t>-57.73789452137719</t>
-        </is>
-      </c>
-      <c r="AW8" t="inlineStr">
-        <is>
-          <t>-30.84903314524001</t>
-        </is>
-      </c>
-      <c r="AZ8" t="inlineStr">
-        <is>
-          <t>waypoints1_9</t>
+          <t>S30.850695° W57.750220°</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>waypoints2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>waypoints2_1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>-57.77100160681348</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>-30.83932008679283</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>waypoints2_2</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>-57.76266548241949</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>-30.84427984353469</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>waypoints2_3</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>-57.76929218975403</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>-30.8476561435724</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>waypoints2_4</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>-57.76179722313178</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>-30.85090524367848</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>waypoints2_5</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>-57.76795110768024</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>-30.85473965188864</t>
+          <t>Lines</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>waypoints3</t>
+          <t>waypoints1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>waypoints3_1</t>
+          <t>waypoints1_1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>-57.76250104661913</t>
+          <t>-57.74591030449292</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>-30.86874371631878</t>
+          <t>-30.84191223192256</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>waypoints3_2</t>
+          <t>waypoints1_2</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>-57.76065794555369</t>
+          <t>-57.7328311040636</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-30.86592183734532</t>
+          <t>-30.84814365439827</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>waypoints3_3</t>
+          <t>waypoints1_3</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>-57.75627829937304</t>
+          <t>-57.73314345725397</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>-30.86976736416804</t>
+          <t>-30.8539877149353</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>waypoints1_4</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>-57.73542685741717</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>-30.86169653128272</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>waypoints1_5</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>-57.7408503849196</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>-30.86035901665188</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>waypoints1_6</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>-57.73549932725664</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>-30.85579893507902</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>waypoints1_7</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>-57.74177445486709</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>-30.85506639734164</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>waypoints1_8</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>-57.7355574257188</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>-30.85281788159316</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>-57.74124633025218</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t>-30.85041651641221</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>waypoints1_10</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
+          <t>-57.74690239008397</t>
+        </is>
+      </c>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>-30.85374166882512</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>waypoints1_11</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>-57.74701342335079</t>
+        </is>
+      </c>
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>-30.85384714723152</t>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>waypoints1_12</t>
+        </is>
+      </c>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>-57.74906400692047</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>-30.8481931267192</t>
+        </is>
+      </c>
+      <c r="AL10" t="inlineStr">
+        <is>
+          <t>waypoints1_13</t>
+        </is>
+      </c>
+      <c r="AM10" t="inlineStr">
+        <is>
+          <t>-57.74462108277138</t>
+        </is>
+      </c>
+      <c r="AN10" t="inlineStr">
+        <is>
+          <t>-30.84793624415745</t>
+        </is>
+      </c>
+      <c r="AO10" t="inlineStr">
+        <is>
+          <t>waypoints1_14</t>
+        </is>
+      </c>
+      <c r="AP10" t="inlineStr">
+        <is>
+          <t>-57.74887913878435</t>
+        </is>
+      </c>
+      <c r="AQ10" t="inlineStr">
+        <is>
+          <t>-30.84464624755162</t>
+        </is>
+      </c>
+      <c r="AR10" t="inlineStr">
+        <is>
+          <t>waypoints1_15</t>
+        </is>
+      </c>
+      <c r="AS10" t="inlineStr">
+        <is>
+          <t>-57.73937946143569</t>
+        </is>
+      </c>
+      <c r="AT10" t="inlineStr">
+        <is>
+          <t>-30.84663672177698</t>
+        </is>
+      </c>
+      <c r="AU10" t="inlineStr">
+        <is>
+          <t>waypoints1_16</t>
+        </is>
+      </c>
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>-57.73789452137719</t>
+        </is>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>-30.84903314524001</t>
+        </is>
+      </c>
+      <c r="AZ10" t="inlineStr">
+        <is>
+          <t>waypoints1_9</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Shapes</t>
+          <t>waypoints2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>waypoints2_1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>-57.77100160681348</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>-30.83932008679283</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>waypoints2_2</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-57.76266548241949</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-30.84427984353469</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>waypoints2_3</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-57.76929218975403</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>-30.8476561435724</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>waypoints2_4</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>-57.76179722313178</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>-30.85090524367848</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>waypoints2_5</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>-57.76795110768024</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>-30.85473965188864</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>shape1</t>
+          <t>waypoints3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>shape1_1</t>
+          <t>waypoints3_1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>-57.77009709727746</t>
+          <t>-57.76250104661913</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>-30.8630625955768</t>
+          <t>-30.86874371631878</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>shape1_2</t>
+          <t>waypoints3_2</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-57.76604921781347</t>
+          <t>-57.76065794555369</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>-30.86553506657824</t>
+          <t>-30.86592183734532</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>shape1_3</t>
+          <t>waypoints3_3</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>-57.761897862339</t>
+          <t>-57.75627829937304</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>-30.86392027799102</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>shape1_4</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>-57.76316319505478</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>-30.85947493540245</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>shape1_5</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>-57.76990874560585</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>-30.85825450101394</t>
+          <t>-30.86976736416804</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>shape2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>shape2_1</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>-57.75923068215288</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>-30.83907581980194</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>shape2_2</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-57.75586379095699</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-30.83697843296341</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>shape2_3</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>-57.75269227704061</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>-30.8409077598212</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>shape2_4</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>-57.75358160984476</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>-30.83602571430277</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>shape2_5</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>-57.74965981837386</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>-30.8341049252744</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>shape2_6</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>-57.75379043973948</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>-30.83305634841427</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>shape2_7</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>-57.75524233257195</t>
-        </is>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>-30.82723877783867</t>
-        </is>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>shape2_8</t>
-        </is>
-      </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>-57.75695338636017</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>-30.83255891840698</t>
-        </is>
-      </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>-57.76175512226109</t>
-        </is>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>-30.83081996081187</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>shape2_10</t>
-        </is>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>-57.7582165018977</t>
-        </is>
-      </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>-30.83501146578525</t>
-        </is>
-      </c>
-      <c r="AZ13" t="inlineStr">
-        <is>
-          <t>shape2_9</t>
+          <t>Shapes</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>shape1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>shape1_1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>-57.77009709727746</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>-30.8630625955768</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>shape1_2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-57.76604921781347</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-30.86553506657824</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>shape1_3</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-57.761897862339</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>-30.86392027799102</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>shape1_4</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>-57.76316319505478</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>-30.85947493540245</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>shape1_5</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>-57.76990874560585</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>-30.85825450101394</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>shape2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>shape2_1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>-57.75923068215288</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>-30.83907581980194</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>shape2_2</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-57.75586379095699</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-30.83697843296341</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>shape2_3</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-57.75269227704061</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>-30.8409077598212</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>shape2_4</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>-57.75358160984476</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>-30.83602571430277</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>shape2_5</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>-57.74965981837386</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>-30.8341049252744</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>shape2_6</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>-57.75379043973949</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>-30.83305634841427</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>shape2_7</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>-57.75524233257195</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>-30.82723877783867</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>shape2_8</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>-57.75695338636017</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>-30.83255891840698</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>-57.7617551222611</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>-30.83081996081187</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>shape2_10</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>-57.7582165018977</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>-30.83501146578525</t>
+        </is>
+      </c>
+      <c r="AZ15" t="inlineStr">
+        <is>
+          <t>shape2_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>shape3</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>shape3_1</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>-57.74806755516322</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>-30.86678300706145</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>shape3_2</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>-57.74459456018673</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>-30.86690881175097</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>shape3_3</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>-57.74443394351941</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>-30.86409827796442</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>shape3_4</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>-57.74351774932654</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>-30.86392859255302</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>shape3_5</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>-57.74599398560416</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>-30.86177549376765</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>shape3_6</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>-57.74877041005693</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>-30.86387889729891</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="T16" t="inlineStr">
         <is>
           <t>shape3_7</t>
         </is>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="U16" t="inlineStr">
         <is>
           <t>-57.74786850965633</t>
         </is>
       </c>
-      <c r="V14" t="inlineStr">
+      <c r="V16" t="inlineStr">
         <is>
           <t>-30.86392847291402</t>
         </is>
@@ -1321,7 +1375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1339,7 +1393,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 SU col</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1351,7 +1405,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 AA BA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1363,7 +1417,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 SA RD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1375,7 +1429,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 AA DE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1393,6 +1447,30 @@
       <c r="B6" t="inlineStr">
         <is>
           <t>S30.863972° W57.752296°</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6 col</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>S30.859553° W57.743856°</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7 Col</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>S30.850695° W57.750220°</t>
         </is>
       </c>
     </row>

</xml_diff>